<commit_message>
test voor excel file
</commit_message>
<xml_diff>
--- a/inschrijven/inschrijfformulier.xlsx
+++ b/inschrijven/inschrijfformulier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saskia.moens\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xtrip\Documents\GitHub\SidhartaProject\inschrijven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DA164BE-4554-4264-9DA6-1BF71B691640}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1AB6C9-C8DA-4658-AEAD-ABB5B6664E89}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{633561A0-F7AD-40FA-A09A-999B82E7B30C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{633561A0-F7AD-40FA-A09A-999B82E7B30C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>extra info waarvan Dansgroep Sidharta moet op de hoogte zijn:</t>
   </si>
   <si>
-    <t xml:space="preserve">en zal op jaarbasis €200 (*) storten op rekeningnummer BE40 1030 1789 6063 </t>
-  </si>
-  <si>
     <t xml:space="preserve">      indien de danser wil deelnemen aan de supplémentaire technieklessen is er een toestag van €50.</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>INSCHRIJVINGSFORMULIER DANSLESSEN - terug te sturen naar gieleninge@yahoo.com</t>
+  </si>
+  <si>
+    <t>en zal op jaarbasis €200 (*) storten op rekeningnummer BE40 1030 1789 6063</t>
   </si>
 </sst>
 </file>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -430,98 +430,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E38206-140B-4170-BFE2-F2FD52A25AAE}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
+  <sheetProtection insertRows="0"/>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="1yPmYUqPkdmpkPRpKVzqjcYVXuflzaK/ub6k9nbuseQ3dsX7Jbwx1MkP6hinJA6XHoMjcVPkvFkUiM03Db5KBA==" saltValue="7C/WvAXoLfpZ77wsZ4QFFw==" spinCount="100000" sqref="A1:A1048576" name="Plage1"/>
+  </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>